<commit_message>
Version used in first revision for Nature Communications.
</commit_message>
<xml_diff>
--- a/CountryAssumptions.xlsx
+++ b/CountryAssumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chalmers-my.sharepoint.com/personal/morfeldt_chalmers_se/Documents/FairShareforSweden/RScripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morfeldt/Documents/RGItHub/AdditionalCarbonAccountability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{8E0B4267-AA73-6A4E-BEE4-3E213ADB6A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDD50D34-AAE8-42D7-BEBD-BEF2F368F65A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01302BA1-11AD-F445-BA05-241295CB326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EC95B6F3-EE61-4D48-8BC5-E94CF24AFC95}"/>
+    <workbookView xWindow="20000" yWindow="500" windowWidth="13600" windowHeight="20500" xr2:uid="{EC95B6F3-EE61-4D48-8BC5-E94CF24AFC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
@@ -288,7 +288,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,13 +330,13 @@
       <sz val="9"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -453,9 +453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -493,7 +493,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -599,7 +599,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,18 +752,18 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -783,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21.75">
+    <row r="2" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -806,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21.75">
+    <row r="3" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -852,7 +852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21.75">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -875,7 +875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="21.75">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -898,7 +898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21.75">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -921,7 +921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="21.75">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -944,7 +944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -967,7 +967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="21.75">
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -990,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="21.75">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="21.75">
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21.75">
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21.75">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1082,12 +1082,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="21.75">
+    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4">
         <v>1.48</v>
@@ -1105,7 +1105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="21.75">
+    <row r="17" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21.75">
+    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="21.75">
+    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="21.75">
+    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21.75">
+    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="21.75">
+    <row r="22" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="21.75">
+    <row r="23" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="21.75">
+    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="21.75">
+    <row r="25" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="21.75">
+    <row r="26" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="21.75">
+    <row r="27" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="21.75">
+    <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="21.75">
+    <row r="30" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="53.25">
+    <row r="31" spans="1:7" ht="66" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="21.75">
+    <row r="33" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="21.75">
+    <row r="34" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="21.75">
+    <row r="35" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>71</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="21.75">
+    <row r="36" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21.75">
+    <row r="37" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>74</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="21.75">
+    <row r="38" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>76</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>80</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Code used for Revision 2 of the article
</commit_message>
<xml_diff>
--- a/CountryAssumptions.xlsx
+++ b/CountryAssumptions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morfeldt/Documents/RGItHub/AdditionalCarbonAccountability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01302BA1-11AD-F445-BA05-241295CB326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10FCA6C-3D94-2640-A124-141C9CD82DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20000" yWindow="500" windowWidth="13600" windowHeight="20500" xr2:uid="{EC95B6F3-EE61-4D48-8BC5-E94CF24AFC95}"/>
+    <workbookView xWindow="31880" yWindow="4240" windowWidth="13600" windowHeight="20500" xr2:uid="{EC95B6F3-EE61-4D48-8BC5-E94CF24AFC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60B4B17-F21D-E049-AD81-1E51A621823A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1110,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4">
         <v>1.25</v>
@@ -1363,7 +1363,7 @@
         <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C27" s="4">
         <v>0.2</v>

</xml_diff>